<commit_message>
Update Microcontroller Team Noobcoder Protocol.xlsx
</commit_message>
<xml_diff>
--- a/Microcontroller Team Noobcoder Protocol.xlsx
+++ b/Microcontroller Team Noobcoder Protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swift\Documents\GitHub\winter20-21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iqbal\Documents\GitHub\winter20-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D6E158-C8EA-4FBE-AE74-22E0A95847EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D5CC92-2C21-47E4-A84F-6B01E8B3CC4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Microcontroller Team 1</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Coding and connecting circuit through TinkerCAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> State Diagram for Pedestrian And Car TLS</t>
   </si>
 </sst>
 </file>
@@ -375,64 +378,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>

</xml_diff>